<commit_message>
modified kat v2 spreadsheet
</commit_message>
<xml_diff>
--- a/projects/Kat_v2.xlsx
+++ b/projects/Kat_v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="40536" windowHeight="12816" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26260" windowHeight="26640" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Outputs!$A$2:$G$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$2:$AA$5</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1764,9 +1764,6 @@
     <t>pgtol</t>
   </si>
   <si>
-    <t>run_openstudio_workflow_monthly.rb</t>
-  </si>
-  <si>
     <t>cooling_electricity_jan</t>
   </si>
   <si>
@@ -1842,9 +1839,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>1.3.0</t>
-  </si>
-  <si>
     <t>Kats model v2</t>
   </si>
   <si>
@@ -1857,9 +1851,6 @@
     <t>[0.33,0.33,0.33]</t>
   </si>
   <si>
-    <t>0.1.13</t>
-  </si>
-  <si>
     <t>Delta X</t>
   </si>
   <si>
@@ -1867,6 +1858,15 @@
   </si>
   <si>
     <t>AdjustThermostatSetpointsByDegrees</t>
+  </si>
+  <si>
+    <t>0.2.0</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>run_openstudio_workflow.rb</t>
   </si>
 </sst>
 </file>
@@ -1997,8 +1997,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1395">
+  <cellStyleXfs count="1399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3469,7 +3473,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1395">
+  <cellStyles count="1399">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4167,6 +4171,8 @@
     <cellStyle name="Followed Hyperlink" xfId="1390" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1392" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1398" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4864,6 +4870,8 @@
     <cellStyle name="Hyperlink" xfId="1389" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1391" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1397" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5169,17 +5177,17 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -5199,21 +5207,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="20"/>
       <c r="B1" s="25"/>
       <c r="C1" s="20"/>
@@ -5222,7 +5230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="13" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>441</v>
       </c>
@@ -5231,18 +5239,18 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>442</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="28">
       <c r="A4" s="1" t="s">
         <v>475</v>
       </c>
@@ -5253,18 +5261,18 @@
         <v>476</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28">
       <c r="A5" s="1" t="s">
         <v>493</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="56">
       <c r="A6" s="1" t="s">
         <v>495</v>
       </c>
@@ -5275,7 +5283,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>455</v>
       </c>
@@ -5294,7 +5302,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28">
       <c r="A8" s="1" t="s">
         <v>456</v>
       </c>
@@ -5313,12 +5321,12 @@
         <v>458</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>477</v>
       </c>
       <c r="B9" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -5326,7 +5334,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="13" customFormat="1">
       <c r="A11" s="12" t="s">
         <v>31</v>
       </c>
@@ -5335,18 +5343,18 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -5357,7 +5365,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -5365,7 +5373,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>486</v>
       </c>
@@ -5376,7 +5384,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>487</v>
       </c>
@@ -5387,7 +5395,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>488</v>
       </c>
@@ -5398,21 +5406,21 @@
         <v>443</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>490</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="32" customFormat="1">
       <c r="B19" s="33"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="56">
       <c r="A20" s="12" t="s">
         <v>30</v>
       </c>
@@ -5423,7 +5431,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>470</v>
       </c>
@@ -5431,7 +5439,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="56">
       <c r="A23" s="12" t="s">
         <v>466</v>
       </c>
@@ -5442,7 +5450,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -5450,7 +5458,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -5458,7 +5466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>573</v>
       </c>
@@ -5466,7 +5474,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>577</v>
       </c>
@@ -5474,7 +5482,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
         <v>574</v>
       </c>
@@ -5482,7 +5490,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>576</v>
       </c>
@@ -5490,10 +5498,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5">
       <c r="B30" s="31"/>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A31" s="12" t="s">
         <v>36</v>
       </c>
@@ -5506,7 +5514,7 @@
       <c r="D31" s="12"/>
       <c r="E31" s="14"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
@@ -5514,7 +5522,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="28">
       <c r="A34" s="12" t="s">
         <v>33</v>
       </c>
@@ -5531,12 +5539,12 @@
         <v>463</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="28">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>46</v>
@@ -5548,7 +5556,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="42">
       <c r="A37" s="12" t="s">
         <v>38</v>
       </c>
@@ -5592,35 +5600,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="47" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.1640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="6.6640625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="7.77734375" style="1" customWidth="1"/>
-    <col min="16" max="19" width="11.44140625" style="1"/>
-    <col min="20" max="20" width="46.109375" style="1" customWidth="1"/>
-    <col min="21" max="23" width="11.44140625" style="1"/>
+    <col min="14" max="15" width="7.83203125" style="1" customWidth="1"/>
+    <col min="16" max="19" width="11.5" style="1"/>
+    <col min="20" max="20" width="46.1640625" style="1" customWidth="1"/>
+    <col min="21" max="23" width="11.5" style="1"/>
     <col min="24" max="24" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="11.44140625" style="1"/>
+    <col min="25" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -5656,7 +5664,7 @@
       <c r="Y1" s="34"/>
       <c r="Z1" s="34"/>
     </row>
-    <row r="2" spans="1:26" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -5669,12 +5677,12 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:26" s="15" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" s="15" customFormat="1" ht="45">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>28</v>
@@ -5713,7 +5721,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="17" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="P3" s="17" t="s">
         <v>503</v>
@@ -5746,7 +5754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26">
       <c r="A4" s="1" t="b">
         <v>0</v>
       </c>
@@ -5757,7 +5765,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26">
       <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
@@ -5779,7 +5787,7 @@
       <c r="O5" s="3"/>
       <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" customFormat="1" ht="15">
       <c r="A6" s="18" t="b">
         <v>1</v>
       </c>
@@ -5787,10 +5795,10 @@
         <v>193</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>74</v>
@@ -5808,7 +5816,7 @@
       <c r="P6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" customFormat="1" ht="15">
       <c r="A7" s="18"/>
       <c r="B7" s="18" t="s">
         <v>25</v>
@@ -5843,16 +5851,16 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="Q7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" customFormat="1" ht="15">
       <c r="A8" s="18"/>
       <c r="B8" s="18" t="s">
         <v>25</v>
@@ -5887,16 +5895,16 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="Q8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" customFormat="1" ht="15">
       <c r="A9" s="18"/>
       <c r="B9" s="18" t="s">
         <v>24</v>
@@ -5945,18 +5953,18 @@
       <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.44140625" style="1"/>
+    <col min="7" max="16384" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="18">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="8" t="s">
@@ -5967,7 +5975,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
         <v>479</v>
       </c>
@@ -5987,7 +5995,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="15" customFormat="1" ht="15">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
@@ -5999,7 +6007,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>568</v>
       </c>
@@ -6018,7 +6026,7 @@
       <c r="F4"/>
       <c r="G4"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>570</v>
       </c>
@@ -6037,15 +6045,15 @@
       <c r="F5"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -6059,15 +6067,15 @@
       </c>
       <c r="G6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B7" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C7" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -6081,15 +6089,15 @@
       </c>
       <c r="G7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B8" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -6103,15 +6111,15 @@
       </c>
       <c r="G8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C9" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -6125,15 +6133,15 @@
       </c>
       <c r="G9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -6147,15 +6155,15 @@
       </c>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -6169,15 +6177,15 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B12" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -6191,15 +6199,15 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C13" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -6213,15 +6221,15 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B14" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C14" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -6235,15 +6243,15 @@
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" customFormat="1">
       <c r="A15" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B15" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C15" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -6256,15 +6264,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" customFormat="1">
       <c r="A16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="C16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -6277,15 +6285,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" customFormat="1">
       <c r="A17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B17" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -6298,15 +6306,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" customFormat="1">
       <c r="A18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B18" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C18" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -6319,15 +6327,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" customFormat="1">
       <c r="A19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C19" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -6340,15 +6348,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" customFormat="1">
       <c r="A20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B20" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C20" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -6361,15 +6369,15 @@
         <v>46320380000</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B21" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C21" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -6383,15 +6391,15 @@
       </c>
       <c r="G21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B22" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C22" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
@@ -6405,15 +6413,15 @@
       </c>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
@@ -6427,15 +6435,15 @@
       </c>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -6449,15 +6457,15 @@
       </c>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B25" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C25" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
@@ -6471,15 +6479,15 @@
       </c>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C26" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
@@ -6493,15 +6501,15 @@
       </c>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B27" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C27" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -6515,15 +6523,15 @@
       </c>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B28" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C28" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -6537,15 +6545,15 @@
       </c>
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
+        <v>601</v>
+      </c>
+      <c r="B29" t="s">
+        <v>601</v>
+      </c>
+      <c r="C29" t="s">
         <v>602</v>
-      </c>
-      <c r="B29" t="s">
-        <v>602</v>
-      </c>
-      <c r="C29" t="s">
-        <v>603</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -6559,7 +6567,7 @@
       </c>
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -6587,19 +6595,19 @@
       <selection sqref="A1:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15">
       <c r="A1" s="18" t="b">
         <v>0</v>
       </c>
@@ -6618,7 +6626,7 @@
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
         <v>24</v>
@@ -6639,7 +6647,7 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
         <v>24</v>
@@ -6662,7 +6670,7 @@
       </c>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
         <v>24</v>
@@ -6685,7 +6693,7 @@
       </c>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
         <v>24</v>
@@ -6708,7 +6716,7 @@
       </c>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
         <v>24</v>
@@ -6731,7 +6739,7 @@
       </c>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15">
       <c r="A7" s="18"/>
       <c r="B7" s="18" t="s">
         <v>24</v>
@@ -6754,7 +6762,7 @@
       </c>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="18"/>
       <c r="B8" s="18" t="s">
         <v>24</v>
@@ -6777,7 +6785,7 @@
       </c>
       <c r="I8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="18"/>
       <c r="B9" s="18" t="s">
         <v>24</v>
@@ -6800,7 +6808,7 @@
       </c>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="18"/>
       <c r="B10" s="18" t="s">
         <v>24</v>
@@ -6823,7 +6831,7 @@
       </c>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15">
       <c r="A11" s="18" t="b">
         <v>0</v>
       </c>
@@ -6842,7 +6850,7 @@
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" s="18"/>
       <c r="B12" s="18" t="s">
         <v>24</v>
@@ -6863,7 +6871,7 @@
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15">
       <c r="A13" s="18"/>
       <c r="B13" s="18" t="s">
         <v>24</v>
@@ -6886,7 +6894,7 @@
       </c>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="18"/>
       <c r="B14" s="18" t="s">
         <v>24</v>
@@ -6909,7 +6917,7 @@
       </c>
       <c r="I14" s="18"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15">
       <c r="A15" s="18"/>
       <c r="B15" s="18" t="s">
         <v>24</v>
@@ -6932,7 +6940,7 @@
       </c>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15">
       <c r="A16" s="18"/>
       <c r="B16" s="18" t="s">
         <v>24</v>
@@ -6955,7 +6963,7 @@
       </c>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15">
       <c r="A17" s="18"/>
       <c r="B17" s="18" t="s">
         <v>24</v>
@@ -6978,7 +6986,7 @@
       </c>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15">
       <c r="A18" s="18"/>
       <c r="B18" s="18" t="s">
         <v>24</v>
@@ -7001,7 +7009,7 @@
       </c>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15">
       <c r="A19" s="18"/>
       <c r="B19" s="18" t="s">
         <v>24</v>
@@ -7024,7 +7032,7 @@
       </c>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15">
       <c r="A20" s="18"/>
       <c r="B20" s="18" t="s">
         <v>24</v>
@@ -7047,7 +7055,7 @@
       </c>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15">
       <c r="A21" s="18" t="b">
         <v>0</v>
       </c>
@@ -7066,7 +7074,7 @@
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15">
       <c r="A22" s="18"/>
       <c r="B22" s="18" t="s">
         <v>24</v>
@@ -7089,7 +7097,7 @@
       </c>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15">
       <c r="A23" s="18"/>
       <c r="B23" s="18" t="s">
         <v>24</v>
@@ -7112,7 +7120,7 @@
       </c>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15">
       <c r="A24" s="18"/>
       <c r="B24" s="18" t="s">
         <v>24</v>
@@ -7135,7 +7143,7 @@
       </c>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15">
       <c r="A25" s="18"/>
       <c r="B25" s="18" t="s">
         <v>24</v>
@@ -7158,7 +7166,7 @@
       </c>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15">
       <c r="A26" s="18"/>
       <c r="B26" s="18" t="s">
         <v>24</v>
@@ -7181,7 +7189,7 @@
       </c>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15">
       <c r="A27" s="18"/>
       <c r="B27" s="18" t="s">
         <v>24</v>
@@ -7204,7 +7212,7 @@
       </c>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15">
       <c r="A28" s="18"/>
       <c r="B28" s="18" t="s">
         <v>24</v>
@@ -7227,7 +7235,7 @@
       </c>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15">
       <c r="A29" s="18"/>
       <c r="B29" s="18" t="s">
         <v>24</v>
@@ -7250,7 +7258,7 @@
       </c>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15">
       <c r="A30" s="18"/>
       <c r="B30" s="18" t="s">
         <v>24</v>
@@ -7273,7 +7281,7 @@
       </c>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15">
       <c r="A31" s="18" t="b">
         <v>0</v>
       </c>
@@ -7292,7 +7300,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15">
       <c r="A32" s="18"/>
       <c r="B32" s="18" t="s">
         <v>24</v>
@@ -7313,7 +7321,7 @@
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15">
       <c r="A33" s="18"/>
       <c r="B33" s="18" t="s">
         <v>24</v>
@@ -7336,7 +7344,7 @@
       </c>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15">
       <c r="A34" s="18"/>
       <c r="B34" s="18" t="s">
         <v>24</v>
@@ -7359,7 +7367,7 @@
       </c>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15">
       <c r="A35" s="18"/>
       <c r="B35" s="18" t="s">
         <v>24</v>
@@ -7382,7 +7390,7 @@
       </c>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15">
       <c r="A36" s="18"/>
       <c r="B36" s="18" t="s">
         <v>24</v>
@@ -7405,7 +7413,7 @@
       </c>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15">
       <c r="A37" s="18"/>
       <c r="B37" s="18" t="s">
         <v>24</v>
@@ -7428,7 +7436,7 @@
       </c>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15">
       <c r="A38" s="18"/>
       <c r="B38" s="18" t="s">
         <v>24</v>
@@ -7451,7 +7459,7 @@
       </c>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15">
       <c r="A39" s="18"/>
       <c r="B39" s="18" t="s">
         <v>24</v>
@@ -7474,7 +7482,7 @@
       </c>
       <c r="I39" s="18"/>
     </row>
-    <row r="40" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15">
       <c r="A40" s="18"/>
       <c r="B40" s="18" t="s">
         <v>24</v>
@@ -7497,7 +7505,7 @@
       </c>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15">
       <c r="A41" s="18" t="b">
         <v>0</v>
       </c>
@@ -7516,7 +7524,7 @@
       <c r="H41" s="18"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15">
       <c r="A42" s="18"/>
       <c r="B42" s="18" t="s">
         <v>24</v>
@@ -7537,7 +7545,7 @@
       <c r="H42" s="18"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15">
       <c r="A43" s="18"/>
       <c r="B43" s="18" t="s">
         <v>24</v>
@@ -7560,7 +7568,7 @@
       </c>
       <c r="I43" s="18"/>
     </row>
-    <row r="44" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15">
       <c r="A44" s="18"/>
       <c r="B44" s="18" t="s">
         <v>24</v>
@@ -7583,7 +7591,7 @@
       </c>
       <c r="I44" s="18"/>
     </row>
-    <row r="45" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15">
       <c r="A45" s="18"/>
       <c r="B45" s="18" t="s">
         <v>24</v>
@@ -7606,7 +7614,7 @@
       </c>
       <c r="I45" s="18"/>
     </row>
-    <row r="46" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15">
       <c r="A46" s="18"/>
       <c r="B46" s="18" t="s">
         <v>24</v>
@@ -7629,7 +7637,7 @@
       </c>
       <c r="I46" s="18"/>
     </row>
-    <row r="47" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15">
       <c r="A47" s="18"/>
       <c r="B47" s="18" t="s">
         <v>24</v>
@@ -7652,7 +7660,7 @@
       </c>
       <c r="I47" s="18"/>
     </row>
-    <row r="48" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15">
       <c r="A48" s="18"/>
       <c r="B48" s="18" t="s">
         <v>24</v>
@@ -7675,7 +7683,7 @@
       </c>
       <c r="I48" s="18"/>
     </row>
-    <row r="49" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15">
       <c r="A49" s="18"/>
       <c r="B49" s="18" t="s">
         <v>24</v>
@@ -7698,7 +7706,7 @@
       </c>
       <c r="I49" s="18"/>
     </row>
-    <row r="50" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15">
       <c r="A50" s="18"/>
       <c r="B50" s="18" t="s">
         <v>24</v>
@@ -7721,7 +7729,7 @@
       </c>
       <c r="I50" s="18"/>
     </row>
-    <row r="51" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15">
       <c r="A51" s="18" t="b">
         <v>0</v>
       </c>
@@ -7740,7 +7748,7 @@
       <c r="H51" s="18"/>
       <c r="I51" s="18"/>
     </row>
-    <row r="52" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15">
       <c r="A52" s="18"/>
       <c r="B52" s="18" t="s">
         <v>24</v>
@@ -7761,7 +7769,7 @@
       <c r="H52" s="18"/>
       <c r="I52" s="18"/>
     </row>
-    <row r="53" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15">
       <c r="A53" s="18"/>
       <c r="B53" s="18" t="s">
         <v>24</v>
@@ -7784,7 +7792,7 @@
       </c>
       <c r="I53" s="18"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15">
       <c r="A54" s="18"/>
       <c r="B54" s="18" t="s">
         <v>24</v>
@@ -7807,7 +7815,7 @@
       </c>
       <c r="I54" s="18"/>
     </row>
-    <row r="55" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15">
       <c r="A55" s="18"/>
       <c r="B55" s="18" t="s">
         <v>24</v>
@@ -7830,7 +7838,7 @@
       </c>
       <c r="I55" s="18"/>
     </row>
-    <row r="56" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15">
       <c r="A56" s="18"/>
       <c r="B56" s="18" t="s">
         <v>24</v>
@@ -7853,7 +7861,7 @@
       </c>
       <c r="I56" s="18"/>
     </row>
-    <row r="57" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15">
       <c r="A57" s="18"/>
       <c r="B57" s="18" t="s">
         <v>24</v>
@@ -7876,7 +7884,7 @@
       </c>
       <c r="I57" s="18"/>
     </row>
-    <row r="58" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15">
       <c r="A58" s="18"/>
       <c r="B58" s="18" t="s">
         <v>24</v>
@@ -7899,7 +7907,7 @@
       </c>
       <c r="I58" s="18"/>
     </row>
-    <row r="59" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15">
       <c r="A59" s="18"/>
       <c r="B59" s="18" t="s">
         <v>24</v>
@@ -7922,7 +7930,7 @@
       </c>
       <c r="I59" s="18"/>
     </row>
-    <row r="60" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15">
       <c r="A60" s="18"/>
       <c r="B60" s="18" t="s">
         <v>24</v>
@@ -7945,7 +7953,7 @@
       </c>
       <c r="I60" s="18"/>
     </row>
-    <row r="61" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15">
       <c r="A61" s="18" t="b">
         <v>0</v>
       </c>
@@ -7964,7 +7972,7 @@
       <c r="H61" s="18"/>
       <c r="I61" s="18"/>
     </row>
-    <row r="62" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15">
       <c r="A62" s="18"/>
       <c r="B62" s="18" t="s">
         <v>24</v>
@@ -7985,7 +7993,7 @@
       <c r="H62" s="18"/>
       <c r="I62" s="18"/>
     </row>
-    <row r="63" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15">
       <c r="A63" s="18"/>
       <c r="B63" s="18" t="s">
         <v>24</v>
@@ -8010,7 +8018,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15">
       <c r="A64" s="18"/>
       <c r="B64" s="18" t="s">
         <v>24</v>
@@ -8033,7 +8041,7 @@
       </c>
       <c r="I64" s="18"/>
     </row>
-    <row r="65" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15">
       <c r="A65" s="18"/>
       <c r="B65" s="18" t="s">
         <v>24</v>
@@ -8056,7 +8064,7 @@
       </c>
       <c r="I65" s="18"/>
     </row>
-    <row r="66" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15">
       <c r="A66" s="18"/>
       <c r="B66" s="18" t="s">
         <v>24</v>
@@ -8079,7 +8087,7 @@
       </c>
       <c r="I66" s="18"/>
     </row>
-    <row r="67" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15">
       <c r="A67" s="18"/>
       <c r="B67" s="18" t="s">
         <v>24</v>
@@ -8102,7 +8110,7 @@
       </c>
       <c r="I67" s="18"/>
     </row>
-    <row r="68" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15">
       <c r="A68" s="18"/>
       <c r="B68" s="18" t="s">
         <v>24</v>
@@ -8125,7 +8133,7 @@
       </c>
       <c r="I68" s="18"/>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15">
       <c r="A69" s="18"/>
       <c r="B69" s="18" t="s">
         <v>24</v>
@@ -8148,7 +8156,7 @@
       </c>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15">
       <c r="A70" s="18"/>
       <c r="B70" s="18" t="s">
         <v>24</v>
@@ -8171,7 +8179,7 @@
       </c>
       <c r="I70" s="18"/>
     </row>
-    <row r="71" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15">
       <c r="A71" s="18"/>
       <c r="B71" s="18" t="s">
         <v>24</v>
@@ -8194,7 +8202,7 @@
       </c>
       <c r="I71" s="18"/>
     </row>
-    <row r="72" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15">
       <c r="A72" s="18" t="b">
         <v>0</v>
       </c>
@@ -8213,7 +8221,7 @@
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
     </row>
-    <row r="73" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15">
       <c r="A73" s="18"/>
       <c r="B73" s="18" t="s">
         <v>24</v>
@@ -8234,7 +8242,7 @@
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
     </row>
-    <row r="74" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15">
       <c r="A74" s="18"/>
       <c r="B74" s="18" t="s">
         <v>24</v>
@@ -8257,7 +8265,7 @@
       </c>
       <c r="I74" s="18"/>
     </row>
-    <row r="75" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15">
       <c r="A75" s="18"/>
       <c r="B75" s="18" t="s">
         <v>24</v>
@@ -8282,7 +8290,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15">
       <c r="A76" s="18"/>
       <c r="B76" s="18" t="s">
         <v>24</v>
@@ -8305,7 +8313,7 @@
       </c>
       <c r="I76" s="18"/>
     </row>
-    <row r="77" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15">
       <c r="A77" s="18"/>
       <c r="B77" s="18" t="s">
         <v>24</v>
@@ -8328,7 +8336,7 @@
       </c>
       <c r="I77" s="18"/>
     </row>
-    <row r="78" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15">
       <c r="A78" s="18"/>
       <c r="B78" s="18" t="s">
         <v>24</v>
@@ -8351,7 +8359,7 @@
       </c>
       <c r="I78" s="18"/>
     </row>
-    <row r="79" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15">
       <c r="A79" s="18"/>
       <c r="B79" s="18" t="s">
         <v>24</v>
@@ -8374,7 +8382,7 @@
       </c>
       <c r="I79" s="18"/>
     </row>
-    <row r="80" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" ht="15">
       <c r="A80" s="18"/>
       <c r="B80" s="18" t="s">
         <v>24</v>
@@ -8397,7 +8405,7 @@
       </c>
       <c r="I80" s="18"/>
     </row>
-    <row r="81" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15">
       <c r="A81" s="18"/>
       <c r="B81" s="18" t="s">
         <v>24</v>
@@ -8420,7 +8428,7 @@
       </c>
       <c r="I81" s="18"/>
     </row>
-    <row r="82" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15">
       <c r="A82" s="18"/>
       <c r="B82" s="18" t="s">
         <v>24</v>
@@ -8443,7 +8451,7 @@
       </c>
       <c r="I82" s="18"/>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15">
       <c r="A83" s="18"/>
       <c r="B83" s="18" t="s">
         <v>24</v>
@@ -8466,7 +8474,7 @@
       </c>
       <c r="I83" s="18"/>
     </row>
-    <row r="84" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15">
       <c r="A84" s="18"/>
       <c r="B84" s="18" t="s">
         <v>24</v>
@@ -8489,7 +8497,7 @@
       </c>
       <c r="I84" s="18"/>
     </row>
-    <row r="85" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" ht="15">
       <c r="A85" s="18"/>
       <c r="B85" s="18" t="s">
         <v>24</v>
@@ -8512,7 +8520,7 @@
       </c>
       <c r="I85" s="18"/>
     </row>
-    <row r="86" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15">
       <c r="A86" s="18" t="b">
         <v>0</v>
       </c>
@@ -8531,7 +8539,7 @@
       <c r="H86" s="18"/>
       <c r="I86" s="18"/>
     </row>
-    <row r="87" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15">
       <c r="A87" s="18"/>
       <c r="B87" s="18" t="s">
         <v>24</v>
@@ -8554,7 +8562,7 @@
       </c>
       <c r="I87" s="18"/>
     </row>
-    <row r="88" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15">
       <c r="A88" s="18"/>
       <c r="B88" s="18" t="s">
         <v>24</v>
@@ -8577,7 +8585,7 @@
       </c>
       <c r="I88" s="18"/>
     </row>
-    <row r="89" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="18"/>
       <c r="B89" s="18" t="s">
         <v>24</v>
@@ -8600,7 +8608,7 @@
       </c>
       <c r="I89" s="18"/>
     </row>
-    <row r="90" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" ht="15">
       <c r="A90" s="18"/>
       <c r="B90" s="18" t="s">
         <v>24</v>
@@ -8623,7 +8631,7 @@
       </c>
       <c r="I90" s="18"/>
     </row>
-    <row r="91" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15">
       <c r="A91" s="18"/>
       <c r="B91" s="18" t="s">
         <v>24</v>
@@ -8646,7 +8654,7 @@
       </c>
       <c r="I91" s="18"/>
     </row>
-    <row r="92" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15">
       <c r="A92" s="18"/>
       <c r="B92" s="18" t="s">
         <v>24</v>
@@ -8669,7 +8677,7 @@
       </c>
       <c r="I92" s="18"/>
     </row>
-    <row r="93" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15">
       <c r="A93" s="18"/>
       <c r="B93" s="18" t="s">
         <v>24</v>
@@ -8692,7 +8700,7 @@
       </c>
       <c r="I93" s="18"/>
     </row>
-    <row r="94" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15">
       <c r="A94" s="18"/>
       <c r="B94" s="18" t="s">
         <v>24</v>
@@ -8715,7 +8723,7 @@
       </c>
       <c r="I94" s="18"/>
     </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15">
       <c r="A95" s="18"/>
       <c r="B95" s="18" t="s">
         <v>24</v>
@@ -8738,7 +8746,7 @@
       </c>
       <c r="I95" s="18"/>
     </row>
-    <row r="96" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" ht="15">
       <c r="A96" s="18"/>
       <c r="B96" s="18" t="s">
         <v>24</v>
@@ -8761,7 +8769,7 @@
       </c>
       <c r="I96" s="18"/>
     </row>
-    <row r="97" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" ht="15">
       <c r="A97" s="18" t="b">
         <v>0</v>
       </c>
@@ -8780,7 +8788,7 @@
       <c r="H97" s="18"/>
       <c r="I97" s="18"/>
     </row>
-    <row r="98" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" ht="15">
       <c r="A98" s="18"/>
       <c r="B98" s="18" t="s">
         <v>24</v>
@@ -8805,7 +8813,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" ht="15">
       <c r="A99" s="18" t="b">
         <v>0</v>
       </c>
@@ -8824,7 +8832,7 @@
       <c r="H99" s="18"/>
       <c r="I99" s="18"/>
     </row>
-    <row r="100" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" ht="15">
       <c r="A100" s="18"/>
       <c r="B100" s="18" t="s">
         <v>24</v>
@@ -8845,7 +8853,7 @@
       <c r="H100" s="18"/>
       <c r="I100" s="18"/>
     </row>
-    <row r="101" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" ht="15">
       <c r="A101" s="18"/>
       <c r="B101" s="18" t="s">
         <v>24</v>
@@ -8870,7 +8878,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15">
       <c r="A102" s="18" t="b">
         <v>0</v>
       </c>
@@ -8889,7 +8897,7 @@
       <c r="H102" s="18"/>
       <c r="I102" s="18"/>
     </row>
-    <row r="103" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" ht="15">
       <c r="A103" s="18"/>
       <c r="B103" s="18" t="s">
         <v>24</v>
@@ -8912,7 +8920,7 @@
       </c>
       <c r="I103" s="18"/>
     </row>
-    <row r="104" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" ht="15">
       <c r="A104" s="18"/>
       <c r="B104" s="18" t="s">
         <v>24</v>
@@ -8937,7 +8945,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" ht="15">
       <c r="A105" s="18"/>
       <c r="B105" s="18" t="s">
         <v>24</v>
@@ -8960,7 +8968,7 @@
       </c>
       <c r="I105" s="18"/>
     </row>
-    <row r="106" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" ht="15">
       <c r="A106" s="18"/>
       <c r="B106" s="18" t="s">
         <v>24</v>
@@ -8981,7 +8989,7 @@
       <c r="H106" s="18"/>
       <c r="I106" s="18"/>
     </row>
-    <row r="107" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" ht="15">
       <c r="A107" s="18" t="b">
         <v>0</v>
       </c>
@@ -9000,7 +9008,7 @@
       <c r="H107" s="18"/>
       <c r="I107" s="18"/>
     </row>
-    <row r="108" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" ht="15">
       <c r="A108" s="18"/>
       <c r="B108" s="18" t="s">
         <v>24</v>
@@ -9025,7 +9033,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15">
       <c r="A109" s="18"/>
       <c r="B109" s="18" t="s">
         <v>24</v>
@@ -9048,7 +9056,7 @@
       </c>
       <c r="I109" s="18"/>
     </row>
-    <row r="110" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" ht="15">
       <c r="A110" s="18"/>
       <c r="B110" s="18" t="s">
         <v>24</v>
@@ -9071,7 +9079,7 @@
       </c>
       <c r="I110" s="18"/>
     </row>
-    <row r="111" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" ht="15">
       <c r="A111" s="18"/>
       <c r="B111" s="18" t="s">
         <v>24</v>
@@ -9094,7 +9102,7 @@
       </c>
       <c r="I111" s="18"/>
     </row>
-    <row r="112" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" ht="15">
       <c r="A112" s="18"/>
       <c r="B112" s="18" t="s">
         <v>24</v>
@@ -9117,7 +9125,7 @@
       </c>
       <c r="I112" s="18"/>
     </row>
-    <row r="113" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" ht="15">
       <c r="A113" s="18"/>
       <c r="B113" s="18" t="s">
         <v>24</v>
@@ -9140,7 +9148,7 @@
       </c>
       <c r="I113" s="18"/>
     </row>
-    <row r="114" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" ht="15">
       <c r="A114" s="18"/>
       <c r="B114" s="18" t="s">
         <v>24</v>
@@ -9163,7 +9171,7 @@
       </c>
       <c r="I114" s="18"/>
     </row>
-    <row r="115" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" ht="15">
       <c r="A115" s="18" t="b">
         <v>0</v>
       </c>
@@ -9182,7 +9190,7 @@
       <c r="H115" s="18"/>
       <c r="I115" s="18"/>
     </row>
-    <row r="116" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" ht="15">
       <c r="A116" s="18"/>
       <c r="B116" s="18" t="s">
         <v>24</v>
@@ -9205,7 +9213,7 @@
       </c>
       <c r="I116" s="18"/>
     </row>
-    <row r="117" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" ht="15">
       <c r="A117" s="18"/>
       <c r="B117" s="18" t="s">
         <v>24</v>
@@ -9228,7 +9236,7 @@
       </c>
       <c r="I117" s="18"/>
     </row>
-    <row r="118" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" ht="15">
       <c r="A118" s="18"/>
       <c r="B118" s="18" t="s">
         <v>24</v>
@@ -9251,7 +9259,7 @@
       </c>
       <c r="I118" s="18"/>
     </row>
-    <row r="119" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" ht="15">
       <c r="A119" s="18" t="b">
         <v>0</v>
       </c>
@@ -9270,7 +9278,7 @@
       <c r="H119" s="18"/>
       <c r="I119" s="18"/>
     </row>
-    <row r="120" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" ht="15">
       <c r="A120" s="18"/>
       <c r="B120" s="18" t="s">
         <v>24</v>
@@ -9293,7 +9301,7 @@
       </c>
       <c r="I120" s="18"/>
     </row>
-    <row r="121" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" ht="15">
       <c r="A121" s="18"/>
       <c r="B121" s="18" t="s">
         <v>24</v>
@@ -9316,7 +9324,7 @@
       </c>
       <c r="I121" s="18"/>
     </row>
-    <row r="122" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" ht="15">
       <c r="A122" s="18"/>
       <c r="B122" s="18" t="s">
         <v>24</v>
@@ -9339,7 +9347,7 @@
       </c>
       <c r="I122" s="18"/>
     </row>
-    <row r="123" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" ht="15">
       <c r="A123" s="18"/>
       <c r="B123" s="18" t="s">
         <v>24</v>
@@ -9362,7 +9370,7 @@
       </c>
       <c r="I123" s="18"/>
     </row>
-    <row r="124" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" ht="15">
       <c r="A124" s="18"/>
       <c r="B124" s="18" t="s">
         <v>24</v>
@@ -9385,7 +9393,7 @@
       </c>
       <c r="I124" s="18"/>
     </row>
-    <row r="125" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" ht="15">
       <c r="A125" s="18"/>
       <c r="B125" s="18" t="s">
         <v>24</v>
@@ -9408,7 +9416,7 @@
       </c>
       <c r="I125" s="18"/>
     </row>
-    <row r="126" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" ht="15">
       <c r="A126" s="18" t="b">
         <v>0</v>
       </c>
@@ -9427,7 +9435,7 @@
       <c r="H126" s="18"/>
       <c r="I126" s="18"/>
     </row>
-    <row r="127" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" ht="15">
       <c r="A127" s="18"/>
       <c r="B127" s="18" t="s">
         <v>24</v>
@@ -9452,7 +9460,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" ht="15">
       <c r="A128" s="18"/>
       <c r="B128" s="18" t="s">
         <v>24</v>
@@ -9475,7 +9483,7 @@
       </c>
       <c r="I128" s="18"/>
     </row>
-    <row r="129" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" ht="15">
       <c r="A129" s="18"/>
       <c r="B129" s="18" t="s">
         <v>24</v>
@@ -9498,7 +9506,7 @@
       </c>
       <c r="I129" s="18"/>
     </row>
-    <row r="130" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" ht="15">
       <c r="A130" s="18"/>
       <c r="B130" s="18" t="s">
         <v>24</v>
@@ -9521,7 +9529,7 @@
       </c>
       <c r="I130" s="18"/>
     </row>
-    <row r="131" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="18"/>
       <c r="B131" s="18" t="s">
         <v>24</v>
@@ -9544,7 +9552,7 @@
       </c>
       <c r="I131" s="18"/>
     </row>
-    <row r="132" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" ht="15">
       <c r="A132" s="18"/>
       <c r="B132" s="18" t="s">
         <v>24</v>
@@ -9567,7 +9575,7 @@
       </c>
       <c r="I132" s="18"/>
     </row>
-    <row r="133" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" ht="15">
       <c r="A133" s="18"/>
       <c r="B133" s="18" t="s">
         <v>24</v>
@@ -9590,7 +9598,7 @@
       </c>
       <c r="I133" s="18"/>
     </row>
-    <row r="134" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" ht="15">
       <c r="A134" s="18"/>
       <c r="B134" s="18" t="s">
         <v>24</v>
@@ -9613,7 +9621,7 @@
       </c>
       <c r="I134" s="18"/>
     </row>
-    <row r="135" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" ht="15">
       <c r="A135" s="18"/>
       <c r="B135" s="18" t="s">
         <v>24</v>
@@ -9636,7 +9644,7 @@
       </c>
       <c r="I135" s="18"/>
     </row>
-    <row r="136" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" ht="15">
       <c r="A136" s="18" t="b">
         <v>0</v>
       </c>
@@ -9655,7 +9663,7 @@
       <c r="H136" s="18"/>
       <c r="I136" s="18"/>
     </row>
-    <row r="137" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" ht="15">
       <c r="A137" s="18"/>
       <c r="B137" s="18" t="s">
         <v>24</v>
@@ -9680,7 +9688,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="138" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" ht="15">
       <c r="A138" s="18"/>
       <c r="B138" s="18" t="s">
         <v>24</v>
@@ -9701,7 +9709,7 @@
       <c r="H138" s="18"/>
       <c r="I138" s="18"/>
     </row>
-    <row r="139" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" ht="15">
       <c r="A139" s="18"/>
       <c r="B139" s="18" t="s">
         <v>24</v>
@@ -9724,7 +9732,7 @@
       </c>
       <c r="I139" s="18"/>
     </row>
-    <row r="140" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" ht="15">
       <c r="A140" s="18"/>
       <c r="B140" s="18" t="s">
         <v>24</v>
@@ -9747,7 +9755,7 @@
       </c>
       <c r="I140" s="18"/>
     </row>
-    <row r="141" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" ht="15">
       <c r="A141" s="18"/>
       <c r="B141" s="18" t="s">
         <v>24</v>
@@ -9770,7 +9778,7 @@
       </c>
       <c r="I141" s="18"/>
     </row>
-    <row r="142" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" ht="15">
       <c r="A142" s="18"/>
       <c r="B142" s="18" t="s">
         <v>24</v>
@@ -9793,7 +9801,7 @@
       </c>
       <c r="I142" s="18"/>
     </row>
-    <row r="143" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" ht="15">
       <c r="A143" s="18"/>
       <c r="B143" s="18" t="s">
         <v>24</v>
@@ -9816,7 +9824,7 @@
       </c>
       <c r="I143" s="18"/>
     </row>
-    <row r="144" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" ht="15">
       <c r="A144" s="18"/>
       <c r="B144" s="18" t="s">
         <v>24</v>
@@ -9839,7 +9847,7 @@
       </c>
       <c r="I144" s="18"/>
     </row>
-    <row r="145" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:9" ht="15">
       <c r="A145" s="18"/>
       <c r="B145" s="18" t="s">
         <v>24</v>
@@ -9862,7 +9870,7 @@
       </c>
       <c r="I145" s="18"/>
     </row>
-    <row r="146" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:9" ht="15">
       <c r="A146" s="18"/>
       <c r="B146" s="18" t="s">
         <v>24</v>
@@ -9885,7 +9893,7 @@
       </c>
       <c r="I146" s="18"/>
     </row>
-    <row r="147" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:9" ht="15">
       <c r="A147" s="18"/>
       <c r="B147" s="18" t="s">
         <v>24</v>
@@ -9908,7 +9916,7 @@
       </c>
       <c r="I147" s="18"/>
     </row>
-    <row r="148" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:9" ht="15">
       <c r="A148" s="18"/>
       <c r="B148" s="18" t="s">
         <v>24</v>
@@ -9931,7 +9939,7 @@
       </c>
       <c r="I148" s="18"/>
     </row>
-    <row r="149" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:9" ht="15">
       <c r="A149" s="18"/>
       <c r="B149" s="18" t="s">
         <v>24</v>
@@ -9954,7 +9962,7 @@
       </c>
       <c r="I149" s="18"/>
     </row>
-    <row r="150" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:9" ht="15">
       <c r="A150" s="18"/>
       <c r="B150" s="18" t="s">
         <v>24</v>
@@ -9977,7 +9985,7 @@
       </c>
       <c r="I150" s="18"/>
     </row>
-    <row r="151" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:9" ht="15">
       <c r="A151" s="18" t="b">
         <v>0</v>
       </c>
@@ -9996,7 +10004,7 @@
       <c r="H151" s="18"/>
       <c r="I151" s="18"/>
     </row>
-    <row r="152" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:9" ht="15">
       <c r="A152" s="18"/>
       <c r="B152" s="18" t="s">
         <v>24</v>
@@ -10019,7 +10027,7 @@
       </c>
       <c r="I152" s="18"/>
     </row>
-    <row r="153" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:9" ht="15">
       <c r="A153" s="18" t="b">
         <v>0</v>
       </c>
@@ -10038,7 +10046,7 @@
       <c r="H153" s="18"/>
       <c r="I153" s="18"/>
     </row>
-    <row r="154" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:9" ht="15">
       <c r="A154" s="18"/>
       <c r="B154" s="18" t="s">
         <v>24</v>
@@ -10061,7 +10069,7 @@
       </c>
       <c r="I154" s="18"/>
     </row>
-    <row r="155" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:9" ht="15">
       <c r="A155" s="18"/>
       <c r="B155" s="18" t="s">
         <v>24</v>
@@ -10084,7 +10092,7 @@
       </c>
       <c r="I155" s="18"/>
     </row>
-    <row r="156" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:9" ht="15">
       <c r="A156" s="18" t="b">
         <v>0</v>
       </c>
@@ -10103,7 +10111,7 @@
       <c r="H156" s="18"/>
       <c r="I156" s="18"/>
     </row>
-    <row r="157" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:9" ht="15">
       <c r="A157" s="18"/>
       <c r="B157" s="18" t="s">
         <v>24</v>
@@ -10128,7 +10136,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:9" ht="15">
       <c r="A158" s="18"/>
       <c r="B158" s="18" t="s">
         <v>24</v>
@@ -10151,7 +10159,7 @@
       </c>
       <c r="I158" s="18"/>
     </row>
-    <row r="159" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:9" ht="15">
       <c r="A159" s="18"/>
       <c r="B159" s="18" t="s">
         <v>24</v>
@@ -10174,7 +10182,7 @@
       </c>
       <c r="I159" s="18"/>
     </row>
-    <row r="160" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:9" ht="15">
       <c r="A160" s="18"/>
       <c r="B160" s="18" t="s">
         <v>24</v>
@@ -10197,7 +10205,7 @@
       </c>
       <c r="I160" s="18"/>
     </row>
-    <row r="161" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:9" ht="15">
       <c r="A161" s="18"/>
       <c r="B161" s="18" t="s">
         <v>24</v>
@@ -10220,7 +10228,7 @@
       </c>
       <c r="I161" s="18"/>
     </row>
-    <row r="162" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:9" ht="15">
       <c r="A162" s="18"/>
       <c r="B162" s="18" t="s">
         <v>24</v>
@@ -10243,7 +10251,7 @@
       </c>
       <c r="I162" s="18"/>
     </row>
-    <row r="163" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:9" ht="15">
       <c r="A163" s="18"/>
       <c r="B163" s="18" t="s">
         <v>24</v>
@@ -10266,7 +10274,7 @@
       </c>
       <c r="I163" s="18"/>
     </row>
-    <row r="164" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:9" ht="15">
       <c r="A164" s="18"/>
       <c r="B164" s="18" t="s">
         <v>24</v>
@@ -10289,7 +10297,7 @@
       </c>
       <c r="I164" s="18"/>
     </row>
-    <row r="165" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:9" ht="15">
       <c r="A165" s="18"/>
       <c r="B165" s="18" t="s">
         <v>24</v>
@@ -10312,7 +10320,7 @@
       </c>
       <c r="I165" s="18"/>
     </row>
-    <row r="166" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:9" ht="15">
       <c r="A166" s="18"/>
       <c r="B166" s="18" t="s">
         <v>24</v>
@@ -10335,7 +10343,7 @@
       </c>
       <c r="I166" s="18"/>
     </row>
-    <row r="167" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:9" ht="15">
       <c r="A167" s="18" t="b">
         <v>0</v>
       </c>
@@ -10354,7 +10362,7 @@
       <c r="H167" s="18"/>
       <c r="I167" s="18"/>
     </row>
-    <row r="168" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:9" ht="15">
       <c r="A168" s="18"/>
       <c r="B168" s="18" t="s">
         <v>24</v>
@@ -10379,7 +10387,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:9" ht="15">
       <c r="A169" s="18"/>
       <c r="B169" s="18" t="s">
         <v>24</v>
@@ -10402,7 +10410,7 @@
       </c>
       <c r="I169" s="18"/>
     </row>
-    <row r="170" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:9" ht="15">
       <c r="A170" s="18"/>
       <c r="B170" s="18" t="s">
         <v>24</v>
@@ -10425,7 +10433,7 @@
       </c>
       <c r="I170" s="18"/>
     </row>
-    <row r="171" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:9" ht="15">
       <c r="A171" s="18"/>
       <c r="B171" s="18" t="s">
         <v>24</v>
@@ -10448,7 +10456,7 @@
       </c>
       <c r="I171" s="18"/>
     </row>
-    <row r="172" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:9" ht="15">
       <c r="A172" s="18"/>
       <c r="B172" s="18" t="s">
         <v>24</v>
@@ -10471,7 +10479,7 @@
       </c>
       <c r="I172" s="18"/>
     </row>
-    <row r="173" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:9" ht="15">
       <c r="A173" s="18"/>
       <c r="B173" s="18" t="s">
         <v>24</v>
@@ -10494,7 +10502,7 @@
       </c>
       <c r="I173" s="18"/>
     </row>
-    <row r="174" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:9" ht="15">
       <c r="A174" s="18"/>
       <c r="B174" s="18" t="s">
         <v>24</v>
@@ -10517,7 +10525,7 @@
       </c>
       <c r="I174" s="18"/>
     </row>
-    <row r="175" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:9" ht="15">
       <c r="A175" s="18"/>
       <c r="B175" s="18" t="s">
         <v>24</v>
@@ -10540,7 +10548,7 @@
       </c>
       <c r="I175" s="18"/>
     </row>
-    <row r="176" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:9" ht="15">
       <c r="A176" s="18"/>
       <c r="B176" s="18" t="s">
         <v>24</v>
@@ -10563,7 +10571,7 @@
       </c>
       <c r="I176" s="18"/>
     </row>
-    <row r="177" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:9" ht="15">
       <c r="A177" s="18"/>
       <c r="B177" s="18" t="s">
         <v>24</v>
@@ -10586,7 +10594,7 @@
       </c>
       <c r="I177" s="18"/>
     </row>
-    <row r="178" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:9" ht="15">
       <c r="A178" s="18" t="b">
         <v>0</v>
       </c>
@@ -10605,7 +10613,7 @@
       <c r="H178" s="18"/>
       <c r="I178" s="18"/>
     </row>
-    <row r="179" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:9" ht="15">
       <c r="A179" s="18"/>
       <c r="B179" s="18" t="s">
         <v>24</v>
@@ -10628,7 +10636,7 @@
       </c>
       <c r="I179" s="18"/>
     </row>
-    <row r="180" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:9" ht="15">
       <c r="A180" s="18"/>
       <c r="B180" s="18" t="s">
         <v>24</v>
@@ -10651,7 +10659,7 @@
       </c>
       <c r="I180" s="18"/>
     </row>
-    <row r="181" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:9" ht="15">
       <c r="A181" s="18"/>
       <c r="B181" s="18" t="s">
         <v>24</v>
@@ -10674,7 +10682,7 @@
       </c>
       <c r="I181" s="18"/>
     </row>
-    <row r="182" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:9" ht="15">
       <c r="A182" s="18"/>
       <c r="B182" s="18" t="s">
         <v>24</v>
@@ -10697,7 +10705,7 @@
       </c>
       <c r="I182" s="18"/>
     </row>
-    <row r="183" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:9" ht="15">
       <c r="A183" s="18" t="b">
         <v>0</v>
       </c>
@@ -10716,7 +10724,7 @@
       <c r="H183" s="18"/>
       <c r="I183" s="18"/>
     </row>
-    <row r="184" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:9" ht="15">
       <c r="A184" s="18"/>
       <c r="B184" s="18" t="s">
         <v>24</v>
@@ -10739,7 +10747,7 @@
       </c>
       <c r="I184" s="18"/>
     </row>
-    <row r="185" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:9" ht="15">
       <c r="A185" s="18"/>
       <c r="B185" s="18" t="s">
         <v>24</v>
@@ -10762,7 +10770,7 @@
       </c>
       <c r="I185" s="18"/>
     </row>
-    <row r="186" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:9" ht="15">
       <c r="A186" s="18"/>
       <c r="B186" s="18" t="s">
         <v>24</v>
@@ -10785,7 +10793,7 @@
       </c>
       <c r="I186" s="18"/>
     </row>
-    <row r="187" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:9" ht="15">
       <c r="A187" s="18"/>
       <c r="B187" s="18" t="s">
         <v>24</v>
@@ -10808,7 +10816,7 @@
       </c>
       <c r="I187" s="18"/>
     </row>
-    <row r="188" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:9" ht="15">
       <c r="A188" s="18" t="b">
         <v>0</v>
       </c>
@@ -10827,7 +10835,7 @@
       <c r="H188" s="18"/>
       <c r="I188" s="18"/>
     </row>
-    <row r="189" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:9" ht="15">
       <c r="A189" s="18"/>
       <c r="B189" s="18" t="s">
         <v>24</v>
@@ -10848,7 +10856,7 @@
       <c r="H189" s="18"/>
       <c r="I189" s="18"/>
     </row>
-    <row r="190" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:9" ht="15">
       <c r="A190" s="18"/>
       <c r="B190" s="18" t="s">
         <v>24</v>
@@ -10871,7 +10879,7 @@
       </c>
       <c r="I190" s="18"/>
     </row>
-    <row r="191" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:9" ht="15">
       <c r="A191" s="18" t="b">
         <v>0</v>
       </c>
@@ -10890,7 +10898,7 @@
       <c r="H191" s="18"/>
       <c r="I191" s="18"/>
     </row>
-    <row r="192" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:9" ht="15">
       <c r="A192" s="18"/>
       <c r="B192" s="18" t="s">
         <v>24</v>
@@ -10913,7 +10921,7 @@
       </c>
       <c r="I192" s="18"/>
     </row>
-    <row r="193" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" ht="15">
       <c r="A193" s="18"/>
       <c r="B193" s="18" t="s">
         <v>24</v>
@@ -10938,7 +10946,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" ht="15">
       <c r="A194" s="18"/>
       <c r="B194" s="18" t="s">
         <v>24</v>
@@ -10959,7 +10967,7 @@
       <c r="H194" s="18"/>
       <c r="I194" s="18"/>
     </row>
-    <row r="195" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" ht="15">
       <c r="A195" s="18"/>
       <c r="B195" s="18" t="s">
         <v>24</v>
@@ -10984,7 +10992,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" ht="15">
       <c r="A196" s="18"/>
       <c r="B196" s="18" t="s">
         <v>24</v>
@@ -11009,7 +11017,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" ht="15">
       <c r="A197" s="18" t="b">
         <v>0</v>
       </c>
@@ -11028,7 +11036,7 @@
       <c r="H197" s="18"/>
       <c r="I197" s="18"/>
     </row>
-    <row r="198" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" ht="15">
       <c r="A198" s="18"/>
       <c r="B198" s="18" t="s">
         <v>24</v>
@@ -11053,7 +11061,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" ht="15">
       <c r="A199" s="18"/>
       <c r="B199" s="18" t="s">
         <v>24</v>
@@ -11076,7 +11084,7 @@
       </c>
       <c r="I199" s="18"/>
     </row>
-    <row r="200" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" ht="15">
       <c r="A200" s="18"/>
       <c r="B200" s="18" t="s">
         <v>24</v>
@@ -11099,7 +11107,7 @@
       </c>
       <c r="I200" s="18"/>
     </row>
-    <row r="201" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" ht="15">
       <c r="A201" s="18"/>
       <c r="B201" s="18" t="s">
         <v>24</v>
@@ -11122,7 +11130,7 @@
       </c>
       <c r="I201" s="18"/>
     </row>
-    <row r="202" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" ht="15">
       <c r="A202" s="18"/>
       <c r="B202" s="18" t="s">
         <v>24</v>
@@ -11145,7 +11153,7 @@
       </c>
       <c r="I202" s="18"/>
     </row>
-    <row r="203" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" ht="15">
       <c r="A203" s="18"/>
       <c r="B203" s="18" t="s">
         <v>24</v>
@@ -11168,7 +11176,7 @@
       </c>
       <c r="I203" s="18"/>
     </row>
-    <row r="204" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:9" ht="15">
       <c r="A204" s="18"/>
       <c r="B204" s="18" t="s">
         <v>24</v>
@@ -11191,7 +11199,7 @@
       </c>
       <c r="I204" s="18"/>
     </row>
-    <row r="205" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" ht="15">
       <c r="A205" s="18"/>
       <c r="B205" s="18" t="s">
         <v>24</v>
@@ -11214,7 +11222,7 @@
       </c>
       <c r="I205" s="18"/>
     </row>
-    <row r="206" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" ht="15">
       <c r="A206" s="18"/>
       <c r="B206" s="18" t="s">
         <v>24</v>
@@ -11237,7 +11245,7 @@
       </c>
       <c r="I206" s="18"/>
     </row>
-    <row r="207" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" ht="15">
       <c r="A207" s="18" t="b">
         <v>0</v>
       </c>
@@ -11256,7 +11264,7 @@
       <c r="H207" s="18"/>
       <c r="I207" s="18"/>
     </row>
-    <row r="208" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" ht="15">
       <c r="A208" s="18"/>
       <c r="B208" s="18" t="s">
         <v>24</v>
@@ -11281,7 +11289,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="209" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:9" ht="15">
       <c r="A209" s="18"/>
       <c r="B209" s="18" t="s">
         <v>24</v>
@@ -11304,7 +11312,7 @@
       </c>
       <c r="I209" s="18"/>
     </row>
-    <row r="210" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:9" ht="15">
       <c r="A210" s="18"/>
       <c r="B210" s="18" t="s">
         <v>24</v>
@@ -11327,7 +11335,7 @@
       </c>
       <c r="I210" s="18"/>
     </row>
-    <row r="211" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:9" ht="15">
       <c r="A211" s="18"/>
       <c r="B211" s="18" t="s">
         <v>24</v>
@@ -11350,7 +11358,7 @@
       </c>
       <c r="I211" s="18"/>
     </row>
-    <row r="212" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:9" ht="15">
       <c r="A212" s="18"/>
       <c r="B212" s="18" t="s">
         <v>24</v>
@@ -11373,7 +11381,7 @@
       </c>
       <c r="I212" s="18"/>
     </row>
-    <row r="213" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:9" ht="15">
       <c r="A213" s="18"/>
       <c r="B213" s="18" t="s">
         <v>24</v>
@@ -11396,7 +11404,7 @@
       </c>
       <c r="I213" s="18"/>
     </row>
-    <row r="214" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:9" ht="15">
       <c r="A214" s="18"/>
       <c r="B214" s="18" t="s">
         <v>24</v>
@@ -11419,7 +11427,7 @@
       </c>
       <c r="I214" s="18"/>
     </row>
-    <row r="215" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:9" ht="15">
       <c r="A215" s="18"/>
       <c r="B215" s="18" t="s">
         <v>24</v>
@@ -11442,7 +11450,7 @@
       </c>
       <c r="I215" s="18"/>
     </row>
-    <row r="216" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:9" ht="15">
       <c r="A216" s="18"/>
       <c r="B216" s="18" t="s">
         <v>24</v>
@@ -11465,7 +11473,7 @@
       </c>
       <c r="I216" s="18"/>
     </row>
-    <row r="217" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:9" ht="15">
       <c r="A217" s="18" t="b">
         <v>0</v>
       </c>
@@ -11484,7 +11492,7 @@
       <c r="H217" s="18"/>
       <c r="I217" s="18"/>
     </row>
-    <row r="218" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:9" ht="15">
       <c r="A218" s="18"/>
       <c r="B218" s="18" t="s">
         <v>24</v>
@@ -11505,7 +11513,7 @@
       <c r="H218" s="18"/>
       <c r="I218" s="18"/>
     </row>
-    <row r="219" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:9" ht="15">
       <c r="A219" s="18"/>
       <c r="B219" s="18" t="s">
         <v>24</v>
@@ -11528,7 +11536,7 @@
       </c>
       <c r="I219" s="18"/>
     </row>
-    <row r="220" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:9" ht="15">
       <c r="A220" s="18"/>
       <c r="B220" s="18" t="s">
         <v>24</v>
@@ -11551,7 +11559,7 @@
       </c>
       <c r="I220" s="18"/>
     </row>
-    <row r="221" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:9" ht="15">
       <c r="A221" s="18"/>
       <c r="B221" s="18" t="s">
         <v>24</v>
@@ -11574,7 +11582,7 @@
       </c>
       <c r="I221" s="18"/>
     </row>
-    <row r="222" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:9" ht="15">
       <c r="A222" s="18"/>
       <c r="B222" s="18" t="s">
         <v>24</v>
@@ -11597,7 +11605,7 @@
       </c>
       <c r="I222" s="18"/>
     </row>
-    <row r="223" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:9" ht="15">
       <c r="A223" s="18"/>
       <c r="B223" s="18" t="s">
         <v>24</v>
@@ -11620,7 +11628,7 @@
       </c>
       <c r="I223" s="18"/>
     </row>
-    <row r="224" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:9" ht="15">
       <c r="A224" s="18"/>
       <c r="B224" s="18" t="s">
         <v>24</v>
@@ -11643,7 +11651,7 @@
       </c>
       <c r="I224" s="18"/>
     </row>
-    <row r="225" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" ht="15">
       <c r="A225" s="18"/>
       <c r="B225" s="18" t="s">
         <v>24</v>
@@ -11666,7 +11674,7 @@
       </c>
       <c r="I225" s="18"/>
     </row>
-    <row r="226" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" ht="15">
       <c r="A226" s="18"/>
       <c r="B226" s="18" t="s">
         <v>24</v>
@@ -11689,7 +11697,7 @@
       </c>
       <c r="I226" s="18"/>
     </row>
-    <row r="227" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" ht="15">
       <c r="A227" s="18"/>
       <c r="B227" s="18" t="s">
         <v>24</v>
@@ -11712,7 +11720,7 @@
       </c>
       <c r="I227" s="18"/>
     </row>
-    <row r="228" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" ht="15">
       <c r="A228" s="18"/>
       <c r="B228" s="18" t="s">
         <v>24</v>
@@ -11735,7 +11743,7 @@
       </c>
       <c r="I228" s="18"/>
     </row>
-    <row r="229" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" ht="15">
       <c r="A229" s="18"/>
       <c r="B229" s="18" t="s">
         <v>24</v>
@@ -11758,7 +11766,7 @@
       </c>
       <c r="I229" s="18"/>
     </row>
-    <row r="230" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" ht="15">
       <c r="A230" s="18"/>
       <c r="B230" s="18" t="s">
         <v>24</v>
@@ -11781,7 +11789,7 @@
       </c>
       <c r="I230" s="18"/>
     </row>
-    <row r="231" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" ht="15">
       <c r="A231" s="18"/>
       <c r="B231" s="18" t="s">
         <v>24</v>
@@ -11804,7 +11812,7 @@
       </c>
       <c r="I231" s="18"/>
     </row>
-    <row r="232" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" ht="15">
       <c r="A232" s="18"/>
       <c r="B232" s="18" t="s">
         <v>24</v>
@@ -11827,7 +11835,7 @@
       </c>
       <c r="I232" s="18"/>
     </row>
-    <row r="233" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" ht="15">
       <c r="A233" s="18"/>
       <c r="B233" s="18" t="s">
         <v>24</v>
@@ -11850,7 +11858,7 @@
       </c>
       <c r="I233" s="18"/>
     </row>
-    <row r="234" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" ht="15">
       <c r="A234" s="18" t="b">
         <v>0</v>
       </c>
@@ -11869,7 +11877,7 @@
       <c r="H234" s="18"/>
       <c r="I234" s="18"/>
     </row>
-    <row r="235" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" ht="15">
       <c r="A235" s="18"/>
       <c r="B235" s="18" t="s">
         <v>24</v>
@@ -11890,7 +11898,7 @@
       <c r="H235" s="18"/>
       <c r="I235" s="18"/>
     </row>
-    <row r="236" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" ht="15">
       <c r="A236" s="18"/>
       <c r="B236" s="18" t="s">
         <v>24</v>
@@ -11913,7 +11921,7 @@
       </c>
       <c r="I236" s="18"/>
     </row>
-    <row r="237" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" ht="15">
       <c r="A237" s="18"/>
       <c r="B237" s="18" t="s">
         <v>24</v>
@@ -11936,7 +11944,7 @@
       </c>
       <c r="I237" s="18"/>
     </row>
-    <row r="238" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" ht="15">
       <c r="A238" s="18"/>
       <c r="B238" s="18" t="s">
         <v>24</v>
@@ -11959,7 +11967,7 @@
       </c>
       <c r="I238" s="18"/>
     </row>
-    <row r="239" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" ht="15">
       <c r="A239" s="18"/>
       <c r="B239" s="18" t="s">
         <v>24</v>
@@ -11982,7 +11990,7 @@
       </c>
       <c r="I239" s="18"/>
     </row>
-    <row r="240" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" ht="15">
       <c r="A240" s="18"/>
       <c r="B240" s="18" t="s">
         <v>24</v>
@@ -12005,7 +12013,7 @@
       </c>
       <c r="I240" s="18"/>
     </row>
-    <row r="241" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:9" ht="15">
       <c r="A241" s="18"/>
       <c r="B241" s="18" t="s">
         <v>24</v>
@@ -12028,7 +12036,7 @@
       </c>
       <c r="I241" s="18"/>
     </row>
-    <row r="242" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" ht="15">
       <c r="A242" s="18"/>
       <c r="B242" s="18" t="s">
         <v>24</v>
@@ -12051,7 +12059,7 @@
       </c>
       <c r="I242" s="18"/>
     </row>
-    <row r="243" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:9" ht="15">
       <c r="A243" s="18"/>
       <c r="B243" s="18" t="s">
         <v>24</v>
@@ -12074,7 +12082,7 @@
       </c>
       <c r="I243" s="18"/>
     </row>
-    <row r="244" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" ht="15">
       <c r="A244" s="18"/>
       <c r="B244" s="18" t="s">
         <v>24</v>
@@ -12097,7 +12105,7 @@
       </c>
       <c r="I244" s="18"/>
     </row>
-    <row r="245" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:9" ht="15">
       <c r="A245" s="18"/>
       <c r="B245" s="18" t="s">
         <v>24</v>
@@ -12120,7 +12128,7 @@
       </c>
       <c r="I245" s="18"/>
     </row>
-    <row r="246" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" ht="15">
       <c r="A246" s="18"/>
       <c r="B246" s="18" t="s">
         <v>24</v>
@@ -12143,7 +12151,7 @@
       </c>
       <c r="I246" s="18"/>
     </row>
-    <row r="247" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" ht="15">
       <c r="A247" s="18"/>
       <c r="B247" s="18" t="s">
         <v>24</v>
@@ -12166,7 +12174,7 @@
       </c>
       <c r="I247" s="18"/>
     </row>
-    <row r="248" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:9" ht="15">
       <c r="A248" s="18"/>
       <c r="B248" s="18" t="s">
         <v>24</v>
@@ -12189,7 +12197,7 @@
       </c>
       <c r="I248" s="18"/>
     </row>
-    <row r="249" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" ht="15">
       <c r="A249" s="18"/>
       <c r="B249" s="18" t="s">
         <v>24</v>
@@ -12212,7 +12220,7 @@
       </c>
       <c r="I249" s="18"/>
     </row>
-    <row r="250" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:9" ht="15">
       <c r="A250" s="18"/>
       <c r="B250" s="18" t="s">
         <v>24</v>
@@ -12235,7 +12243,7 @@
       </c>
       <c r="I250" s="18"/>
     </row>
-    <row r="251" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:9" ht="15">
       <c r="A251" s="18" t="b">
         <v>0</v>
       </c>
@@ -12254,7 +12262,7 @@
       <c r="H251" s="18"/>
       <c r="I251" s="18"/>
     </row>
-    <row r="252" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:9" ht="15">
       <c r="A252" s="18"/>
       <c r="B252" s="18" t="s">
         <v>24</v>
@@ -12279,7 +12287,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="253" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:9" ht="15">
       <c r="A253" s="18"/>
       <c r="B253" s="18" t="s">
         <v>24</v>
@@ -12302,7 +12310,7 @@
       </c>
       <c r="I253" s="18"/>
     </row>
-    <row r="254" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:9" ht="15">
       <c r="A254" s="18"/>
       <c r="B254" s="18" t="s">
         <v>24</v>
@@ -12325,7 +12333,7 @@
       </c>
       <c r="I254" s="18"/>
     </row>
-    <row r="255" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:9" ht="15">
       <c r="A255" s="18"/>
       <c r="B255" s="18" t="s">
         <v>24</v>
@@ -12348,7 +12356,7 @@
       </c>
       <c r="I255" s="18"/>
     </row>
-    <row r="256" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" ht="15">
       <c r="A256" s="18"/>
       <c r="B256" s="18" t="s">
         <v>24</v>
@@ -12371,7 +12379,7 @@
       </c>
       <c r="I256" s="18"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="15">
       <c r="A257" s="18" t="b">
         <v>0</v>
       </c>
@@ -12390,7 +12398,7 @@
       <c r="H257" s="18"/>
       <c r="I257" s="18"/>
     </row>
-    <row r="258" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:9" ht="15">
       <c r="A258" s="18"/>
       <c r="B258" s="18" t="s">
         <v>24</v>
@@ -12415,7 +12423,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="259" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:9" ht="15">
       <c r="A259" s="18"/>
       <c r="B259" s="18" t="s">
         <v>24</v>
@@ -12438,7 +12446,7 @@
       </c>
       <c r="I259" s="18"/>
     </row>
-    <row r="260" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:9" ht="15">
       <c r="A260" s="18" t="b">
         <v>0</v>
       </c>
@@ -12457,7 +12465,7 @@
       <c r="H260" s="18"/>
       <c r="I260" s="18"/>
     </row>
-    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:9" ht="15">
       <c r="A261" s="18" t="b">
         <v>0</v>
       </c>
@@ -12476,7 +12484,7 @@
       <c r="H261" s="18"/>
       <c r="I261" s="18"/>
     </row>
-    <row r="262" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:9" ht="15">
       <c r="A262" s="18" t="b">
         <v>0</v>
       </c>
@@ -12495,7 +12503,7 @@
       <c r="H262" s="18"/>
       <c r="I262" s="18"/>
     </row>
-    <row r="263" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:9" ht="15">
       <c r="A263" s="18"/>
       <c r="B263" s="18" t="s">
         <v>24</v>
@@ -12516,7 +12524,7 @@
       <c r="H263" s="18"/>
       <c r="I263" s="18"/>
     </row>
-    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:9" ht="15">
       <c r="A264" s="18"/>
       <c r="B264" s="18" t="s">
         <v>24</v>
@@ -12539,7 +12547,7 @@
       </c>
       <c r="I264" s="18"/>
     </row>
-    <row r="265" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:9" ht="15">
       <c r="A265" s="18"/>
       <c r="B265" s="18" t="s">
         <v>24</v>
@@ -12562,7 +12570,7 @@
       </c>
       <c r="I265" s="18"/>
     </row>
-    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:9" ht="15">
       <c r="A266" s="18"/>
       <c r="B266" s="18" t="s">
         <v>24</v>
@@ -12585,7 +12593,7 @@
       </c>
       <c r="I266" s="18"/>
     </row>
-    <row r="267" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:9" ht="15">
       <c r="A267" s="18"/>
       <c r="B267" s="18" t="s">
         <v>24</v>
@@ -12608,7 +12616,7 @@
       </c>
       <c r="I267" s="18"/>
     </row>
-    <row r="268" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:9" ht="15">
       <c r="A268" s="18"/>
       <c r="B268" s="18" t="s">
         <v>24</v>
@@ -12631,7 +12639,7 @@
       </c>
       <c r="I268" s="18"/>
     </row>
-    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:9" ht="15">
       <c r="A269" s="18"/>
       <c r="B269" s="18" t="s">
         <v>24</v>
@@ -12654,7 +12662,7 @@
       </c>
       <c r="I269" s="18"/>
     </row>
-    <row r="270" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:9" ht="15">
       <c r="A270" s="18"/>
       <c r="B270" s="18" t="s">
         <v>24</v>
@@ -12677,7 +12685,7 @@
       </c>
       <c r="I270" s="18"/>
     </row>
-    <row r="271" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:9" ht="15">
       <c r="A271" s="18"/>
       <c r="B271" s="18" t="s">
         <v>24</v>
@@ -12700,7 +12708,7 @@
       </c>
       <c r="I271" s="18"/>
     </row>
-    <row r="272" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:9" ht="15">
       <c r="A272" s="18"/>
       <c r="B272" s="18" t="s">
         <v>24</v>
@@ -12723,7 +12731,7 @@
       </c>
       <c r="I272" s="18"/>
     </row>
-    <row r="273" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" ht="15">
       <c r="A273" s="18"/>
       <c r="B273" s="18" t="s">
         <v>24</v>
@@ -12746,7 +12754,7 @@
       </c>
       <c r="I273" s="18"/>
     </row>
-    <row r="274" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" ht="15">
       <c r="A274" s="18" t="b">
         <v>0</v>
       </c>
@@ -12765,7 +12773,7 @@
       <c r="H274" s="18"/>
       <c r="I274" s="18"/>
     </row>
-    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" ht="15">
       <c r="A275" s="18"/>
       <c r="B275" s="18" t="s">
         <v>24</v>
@@ -12788,7 +12796,7 @@
       </c>
       <c r="I275" s="18"/>
     </row>
-    <row r="276" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" ht="15">
       <c r="A276" s="18" t="b">
         <v>0</v>
       </c>
@@ -12807,7 +12815,7 @@
       <c r="H276" s="18"/>
       <c r="I276" s="18"/>
     </row>
-    <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:9" ht="15">
       <c r="A277" s="18"/>
       <c r="B277" s="18" t="s">
         <v>24</v>
@@ -12832,7 +12840,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="278" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" ht="15">
       <c r="A278" s="18"/>
       <c r="B278" s="18" t="s">
         <v>24</v>
@@ -12855,7 +12863,7 @@
       </c>
       <c r="I278" s="18"/>
     </row>
-    <row r="279" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" ht="15">
       <c r="A279" s="18"/>
       <c r="B279" s="18" t="s">
         <v>24</v>
@@ -12878,7 +12886,7 @@
       </c>
       <c r="I279" s="18"/>
     </row>
-    <row r="280" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" ht="15">
       <c r="A280" s="18"/>
       <c r="B280" s="18" t="s">
         <v>24</v>
@@ -12901,7 +12909,7 @@
       </c>
       <c r="I280" s="18"/>
     </row>
-    <row r="281" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" ht="15">
       <c r="A281" s="18"/>
       <c r="B281" s="18" t="s">
         <v>24</v>
@@ -12924,7 +12932,7 @@
       </c>
       <c r="I281" s="18"/>
     </row>
-    <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" ht="15">
       <c r="A282" s="18"/>
       <c r="B282" s="18" t="s">
         <v>24</v>
@@ -12947,7 +12955,7 @@
       </c>
       <c r="I282" s="18"/>
     </row>
-    <row r="283" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" ht="15">
       <c r="A283" s="18"/>
       <c r="B283" s="18" t="s">
         <v>24</v>
@@ -12970,7 +12978,7 @@
       </c>
       <c r="I283" s="18"/>
     </row>
-    <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" ht="15">
       <c r="A284" s="18"/>
       <c r="B284" s="18" t="s">
         <v>24</v>
@@ -12993,7 +13001,7 @@
       </c>
       <c r="I284" s="18"/>
     </row>
-    <row r="285" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" ht="15">
       <c r="A285" s="18"/>
       <c r="B285" s="18" t="s">
         <v>24</v>
@@ -13016,7 +13024,7 @@
       </c>
       <c r="I285" s="18"/>
     </row>
-    <row r="286" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" ht="15">
       <c r="A286" s="18"/>
       <c r="B286" s="18" t="s">
         <v>24</v>
@@ -13039,7 +13047,7 @@
       </c>
       <c r="I286" s="18"/>
     </row>
-    <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" ht="15">
       <c r="A287" s="18"/>
       <c r="B287" s="18" t="s">
         <v>24</v>
@@ -13062,7 +13070,7 @@
       </c>
       <c r="I287" s="18"/>
     </row>
-    <row r="288" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" ht="15">
       <c r="A288" s="18" t="b">
         <v>0</v>
       </c>
@@ -13081,7 +13089,7 @@
       <c r="H288" s="18"/>
       <c r="I288" s="18"/>
     </row>
-    <row r="289" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:9" ht="15">
       <c r="A289" s="18"/>
       <c r="B289" s="18" t="s">
         <v>24</v>
@@ -13104,7 +13112,7 @@
       </c>
       <c r="I289" s="18"/>
     </row>
-    <row r="290" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:9" ht="15">
       <c r="A290" s="18" t="b">
         <v>0</v>
       </c>
@@ -13123,7 +13131,7 @@
       <c r="H290" s="18"/>
       <c r="I290" s="18"/>
     </row>
-    <row r="291" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:9" ht="15">
       <c r="A291" s="18"/>
       <c r="B291" s="18" t="s">
         <v>24</v>
@@ -13144,7 +13152,7 @@
       <c r="H291" s="18"/>
       <c r="I291" s="18"/>
     </row>
-    <row r="292" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:9" ht="15">
       <c r="A292" s="18" t="b">
         <v>0</v>
       </c>
@@ -13163,7 +13171,7 @@
       <c r="H292" s="18"/>
       <c r="I292" s="18"/>
     </row>
-    <row r="293" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:9" ht="15">
       <c r="A293" s="18"/>
       <c r="B293" s="18" t="s">
         <v>24</v>
@@ -13184,7 +13192,7 @@
       <c r="H293" s="18"/>
       <c r="I293" s="18"/>
     </row>
-    <row r="294" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:9" ht="15">
       <c r="A294" s="18" t="b">
         <v>0</v>
       </c>
@@ -13203,7 +13211,7 @@
       <c r="H294" s="18"/>
       <c r="I294" s="18"/>
     </row>
-    <row r="295" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:9" ht="15">
       <c r="A295" s="18"/>
       <c r="B295" s="18" t="s">
         <v>24</v>
@@ -13224,7 +13232,7 @@
       <c r="H295" s="18"/>
       <c r="I295" s="18"/>
     </row>
-    <row r="296" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:9" ht="15">
       <c r="A296" s="18" t="b">
         <v>0</v>
       </c>
@@ -13243,7 +13251,7 @@
       <c r="H296" s="18"/>
       <c r="I296" s="18"/>
     </row>
-    <row r="297" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:9" ht="15">
       <c r="A297" s="18"/>
       <c r="B297" s="18" t="s">
         <v>24</v>
@@ -13266,7 +13274,7 @@
       </c>
       <c r="I297" s="18"/>
     </row>
-    <row r="298" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:9" ht="15">
       <c r="A298" s="18" t="b">
         <v>0</v>
       </c>
@@ -13285,7 +13293,7 @@
       <c r="H298" s="18"/>
       <c r="I298" s="18"/>
     </row>
-    <row r="299" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:9" ht="15">
       <c r="A299" s="18"/>
       <c r="B299" s="18" t="s">
         <v>24</v>
@@ -13310,7 +13318,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="300" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:9" ht="15">
       <c r="A300" s="18"/>
       <c r="B300" s="18" t="s">
         <v>24</v>
@@ -13333,7 +13341,7 @@
       </c>
       <c r="I300" s="18"/>
     </row>
-    <row r="301" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:9" ht="15">
       <c r="A301" s="18"/>
       <c r="B301" s="18" t="s">
         <v>24</v>
@@ -13356,7 +13364,7 @@
       </c>
       <c r="I301" s="18"/>
     </row>
-    <row r="302" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:9" ht="15">
       <c r="A302" s="18"/>
       <c r="B302" s="18" t="s">
         <v>24</v>
@@ -13379,7 +13387,7 @@
       </c>
       <c r="I302" s="18"/>
     </row>
-    <row r="303" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:9" ht="15">
       <c r="A303" s="18"/>
       <c r="B303" s="18" t="s">
         <v>24</v>
@@ -13402,7 +13410,7 @@
       </c>
       <c r="I303" s="18"/>
     </row>
-    <row r="304" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:9" ht="15">
       <c r="A304" s="18"/>
       <c r="B304" s="18" t="s">
         <v>24</v>
@@ -13425,7 +13433,7 @@
       </c>
       <c r="I304" s="18"/>
     </row>
-    <row r="305" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:9" ht="15">
       <c r="A305" s="18"/>
       <c r="B305" s="18" t="s">
         <v>24</v>
@@ -13448,7 +13456,7 @@
       </c>
       <c r="I305" s="18"/>
     </row>
-    <row r="306" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:9" ht="15">
       <c r="A306" s="18"/>
       <c r="B306" s="18" t="s">
         <v>24</v>
@@ -13471,7 +13479,7 @@
       </c>
       <c r="I306" s="18"/>
     </row>
-    <row r="307" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:9" ht="15">
       <c r="A307" s="18"/>
       <c r="B307" s="18" t="s">
         <v>24</v>
@@ -13494,7 +13502,7 @@
       </c>
       <c r="I307" s="18"/>
     </row>
-    <row r="308" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:9" ht="15">
       <c r="A308" s="18" t="b">
         <v>0</v>
       </c>
@@ -13513,7 +13521,7 @@
       <c r="H308" s="18"/>
       <c r="I308" s="18"/>
     </row>
-    <row r="309" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:9" ht="15">
       <c r="A309" s="18"/>
       <c r="B309" s="18" t="s">
         <v>24</v>
@@ -13536,7 +13544,7 @@
       </c>
       <c r="I309" s="18"/>
     </row>
-    <row r="310" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:9" ht="15">
       <c r="A310" s="18"/>
       <c r="B310" s="18" t="s">
         <v>24</v>
@@ -13559,7 +13567,7 @@
       </c>
       <c r="I310" s="18"/>
     </row>
-    <row r="311" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:9" ht="15">
       <c r="A311" s="18"/>
       <c r="B311" s="18" t="s">
         <v>24</v>
@@ -13582,7 +13590,7 @@
       </c>
       <c r="I311" s="18"/>
     </row>
-    <row r="312" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:9" ht="15">
       <c r="A312" s="18"/>
       <c r="B312" s="18" t="s">
         <v>24</v>
@@ -13605,7 +13613,7 @@
       </c>
       <c r="I312" s="18"/>
     </row>
-    <row r="313" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:9" ht="15">
       <c r="A313" s="18" t="b">
         <v>0</v>
       </c>
@@ -13624,7 +13632,7 @@
       <c r="H313" s="18"/>
       <c r="I313" s="18"/>
     </row>
-    <row r="314" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:9" ht="15">
       <c r="A314" s="18"/>
       <c r="B314" s="18" t="s">
         <v>24</v>
@@ -13647,7 +13655,7 @@
       </c>
       <c r="I314" s="18"/>
     </row>
-    <row r="315" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:9" ht="15">
       <c r="A315" s="18"/>
       <c r="B315" s="18" t="s">
         <v>24</v>
@@ -13670,7 +13678,7 @@
       </c>
       <c r="I315" s="18"/>
     </row>
-    <row r="316" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:9" ht="15">
       <c r="A316" s="18"/>
       <c r="B316" s="18" t="s">
         <v>24</v>
@@ -13695,7 +13703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:9" ht="15">
       <c r="A317" s="18" t="b">
         <v>0</v>
       </c>
@@ -13714,7 +13722,7 @@
       <c r="H317" s="18"/>
       <c r="I317" s="18"/>
     </row>
-    <row r="318" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:9" ht="15">
       <c r="A318" s="18"/>
       <c r="B318" s="18" t="s">
         <v>24</v>
@@ -13739,7 +13747,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="319" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:9" ht="15">
       <c r="A319" s="18"/>
       <c r="B319" s="18" t="s">
         <v>24</v>
@@ -13762,7 +13770,7 @@
       </c>
       <c r="I319" s="18"/>
     </row>
-    <row r="320" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:9" ht="15">
       <c r="A320" s="18" t="b">
         <v>0</v>
       </c>
@@ -13781,7 +13789,7 @@
       <c r="H320" s="18"/>
       <c r="I320" s="18"/>
     </row>
-    <row r="321" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:9" ht="15">
       <c r="A321" s="18"/>
       <c r="B321" s="18" t="s">
         <v>24</v>
@@ -13802,7 +13810,7 @@
       <c r="H321" s="18"/>
       <c r="I321" s="18"/>
     </row>
-    <row r="322" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:9" ht="15">
       <c r="A322" s="18"/>
       <c r="B322" s="18" t="s">
         <v>24</v>
@@ -13823,7 +13831,7 @@
       <c r="H322" s="18"/>
       <c r="I322" s="18"/>
     </row>
-    <row r="323" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:9" ht="15">
       <c r="A323" s="18"/>
       <c r="B323" s="18" t="s">
         <v>24</v>
@@ -13846,7 +13854,7 @@
       </c>
       <c r="I323" s="18"/>
     </row>
-    <row r="324" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:9" ht="15">
       <c r="A324" s="18" t="b">
         <v>0</v>
       </c>
@@ -13865,7 +13873,7 @@
       <c r="H324" s="18"/>
       <c r="I324" s="18"/>
     </row>
-    <row r="325" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:9" ht="15">
       <c r="A325" s="18" t="b">
         <v>0</v>
       </c>
@@ -13884,7 +13892,7 @@
       <c r="H325" s="18"/>
       <c r="I325" s="18"/>
     </row>
-    <row r="326" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:9" ht="15">
       <c r="A326" s="18"/>
       <c r="B326" s="18" t="s">
         <v>24</v>
@@ -13909,7 +13917,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="327" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:9" ht="15">
       <c r="A327" s="18"/>
       <c r="B327" s="18" t="s">
         <v>24</v>
@@ -13934,7 +13942,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:9">
       <c r="A328" t="b">
         <v>0</v>
       </c>
@@ -13948,7 +13956,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:9">
       <c r="B329" t="s">
         <v>24</v>
       </c>
@@ -13971,7 +13979,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:9">
       <c r="B330" t="s">
         <v>24</v>
       </c>
@@ -13991,7 +13999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:9">
       <c r="B331" t="s">
         <v>24</v>
       </c>
@@ -14011,7 +14019,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:9">
       <c r="B332" t="s">
         <v>24</v>
       </c>
@@ -14031,7 +14039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:9">
       <c r="B333" t="s">
         <v>24</v>
       </c>
@@ -14048,7 +14056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:9">
       <c r="B334" t="s">
         <v>24</v>
       </c>
@@ -14071,7 +14079,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:9">
       <c r="B335" t="s">
         <v>24</v>
       </c>
@@ -14094,7 +14102,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:9">
       <c r="A336" t="b">
         <v>0</v>
       </c>
@@ -14108,7 +14116,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="337" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:16">
       <c r="B337" t="s">
         <v>24</v>
       </c>
@@ -14131,7 +14139,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:16">
       <c r="B338" t="s">
         <v>24</v>
       </c>
@@ -14154,7 +14162,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="339" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:16">
       <c r="B339" t="s">
         <v>24</v>
       </c>
@@ -14174,7 +14182,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="340" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:16">
       <c r="B340" t="s">
         <v>24</v>
       </c>
@@ -14194,7 +14202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:16">
       <c r="B341" t="s">
         <v>24</v>
       </c>
@@ -14211,7 +14219,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="342" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:16">
       <c r="A342" s="1" t="b">
         <v>0</v>
       </c>
@@ -14237,7 +14245,7 @@
       <c r="O342" s="1"/>
       <c r="P342" s="1"/>
     </row>
-    <row r="343" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:16">
       <c r="A343" s="1"/>
       <c r="B343" t="s">
         <v>24</v>
@@ -14266,7 +14274,7 @@
       <c r="O343" s="1"/>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:16" ht="15">
       <c r="A344" s="18"/>
       <c r="B344" t="s">
         <v>24</v>
@@ -14305,7 +14313,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="345" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:16">
       <c r="A345" t="b">
         <v>0</v>
       </c>
@@ -14319,7 +14327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:16">
       <c r="B346" t="s">
         <v>24</v>
       </c>
@@ -14339,7 +14347,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:16">
       <c r="A347" t="b">
         <v>0</v>
       </c>
@@ -14353,7 +14361,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="348" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:16">
       <c r="B348" t="s">
         <v>24</v>
       </c>
@@ -14373,7 +14381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:16">
       <c r="B349" t="s">
         <v>24</v>
       </c>
@@ -14393,7 +14401,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="350" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:16">
       <c r="B350" t="s">
         <v>24</v>
       </c>
@@ -14413,7 +14421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:16">
       <c r="B351" t="s">
         <v>24</v>
       </c>
@@ -14433,7 +14441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:16">
       <c r="B352" t="s">
         <v>24</v>
       </c>
@@ -14453,7 +14461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:18">
       <c r="B353" t="s">
         <v>24</v>
       </c>
@@ -14473,7 +14481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:18">
       <c r="B354" t="s">
         <v>24</v>
       </c>
@@ -14493,7 +14501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="355" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:18">
       <c r="B355" t="s">
         <v>24</v>
       </c>
@@ -14513,7 +14521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:18">
       <c r="B356" t="s">
         <v>24</v>
       </c>
@@ -14533,7 +14541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:18">
       <c r="A357" t="b">
         <v>0</v>
       </c>
@@ -14547,7 +14555,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="358" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:18">
       <c r="B358" t="s">
         <v>24</v>
       </c>
@@ -14567,7 +14575,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="359" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:18">
       <c r="B359" t="s">
         <v>24</v>
       </c>
@@ -14587,7 +14595,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="360" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:18" s="1" customFormat="1">
       <c r="A360" t="b">
         <v>0</v>
       </c>
@@ -14603,7 +14611,7 @@
       <c r="H360" s="5"/>
       <c r="I360" s="5"/>
     </row>
-    <row r="361" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:18" s="1" customFormat="1">
       <c r="B361" t="s">
         <v>24</v>
       </c>
@@ -14629,7 +14637,7 @@
       <c r="J361"/>
       <c r="K361"/>
     </row>
-    <row r="362" spans="1:18" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:18" s="1" customFormat="1" ht="15">
       <c r="A362" s="18"/>
       <c r="B362" t="s">
         <v>25</v>
@@ -14670,7 +14678,7 @@
       <c r="Q362"/>
       <c r="R362"/>
     </row>
-    <row r="363" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:18">
       <c r="A363" t="b">
         <v>0</v>
       </c>
@@ -14684,7 +14692,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="364" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:18">
       <c r="B364" t="s">
         <v>24</v>
       </c>
@@ -14704,7 +14712,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="365" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:18">
       <c r="A365" t="b">
         <v>0</v>
       </c>
@@ -14718,7 +14726,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="366" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:18">
       <c r="B366" t="s">
         <v>24</v>
       </c>
@@ -14757,13 +14765,13 @@
       <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>454</v>
       </c>
@@ -14774,7 +14782,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>444</v>
       </c>
@@ -14785,7 +14793,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>445</v>
       </c>
@@ -14796,7 +14804,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>452</v>
       </c>
@@ -14807,7 +14815,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>446</v>
       </c>
@@ -14818,17 +14826,17 @@
         <v>451</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>471</v>
       </c>

</xml_diff>